<commit_message>
Use HPP file for memory addresses
</commit_message>
<xml_diff>
--- a/docs/Memory_Sheet.xlsx
+++ b/docs/Memory_Sheet.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="16560" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="16560" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Private Block" sheetId="4" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="78">
   <si>
     <t>Speed Controller</t>
   </si>
@@ -213,6 +213,57 @@
   </si>
   <si>
     <t>ENDIAN</t>
+  </si>
+  <si>
+    <t>SPEED_CONTROLLER_0</t>
+  </si>
+  <si>
+    <t>SPEED_CONTROLLER_1</t>
+  </si>
+  <si>
+    <t>SPEED_CONTROLLER_2</t>
+  </si>
+  <si>
+    <t>SPEED_CONTROLLER_3</t>
+  </si>
+  <si>
+    <t>SPEED_CONTROLLER_4</t>
+  </si>
+  <si>
+    <t>SPEED_CONTROLLER_5</t>
+  </si>
+  <si>
+    <t>SPEED_CONTROLLER_6</t>
+  </si>
+  <si>
+    <t>SPEED_CONTROLLER_7</t>
+  </si>
+  <si>
+    <t>SPEED_CONTROLLER_8</t>
+  </si>
+  <si>
+    <t>SPEED_CONTROLLER_9</t>
+  </si>
+  <si>
+    <t>SPEED_CONTROLLER_10</t>
+  </si>
+  <si>
+    <t>SPEED_CONTROLLER_11</t>
+  </si>
+  <si>
+    <t>SPEED_CONTROLLER_12</t>
+  </si>
+  <si>
+    <t>SPEED_CONTROLLER_13</t>
+  </si>
+  <si>
+    <t>SPEED_CONTROLLER_14</t>
+  </si>
+  <si>
+    <t>SPEED_CONTROLLER_15</t>
+  </si>
+  <si>
+    <t>SPEED CONTROLLER / MOTOR</t>
   </si>
 </sst>
 </file>
@@ -500,7 +551,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -712,6 +763,24 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1002,8 +1071,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R35"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20:R35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -1082,13 +1151,13 @@
         <v>60</v>
       </c>
       <c r="D4" s="47" t="s">
+        <v>47</v>
+      </c>
+      <c r="E4" s="73" t="s">
         <v>48</v>
       </c>
-      <c r="E4" s="47" t="s">
+      <c r="F4" s="47" t="s">
         <v>49</v>
-      </c>
-      <c r="F4" s="47" t="s">
-        <v>47</v>
       </c>
       <c r="G4" s="48"/>
       <c r="H4" s="48"/>
@@ -1801,10 +1870,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R35"/>
+  <dimension ref="A1:R115"/>
   <sheetViews>
-    <sheetView showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -1823,6 +1892,11 @@
       <c r="C2" s="1" t="s">
         <v>50</v>
       </c>
+      <c r="F2" s="75" t="s">
+        <v>77</v>
+      </c>
+      <c r="G2" s="76"/>
+      <c r="H2" s="77"/>
     </row>
     <row r="3" spans="1:18">
       <c r="C3" s="3">
@@ -1876,8 +1950,8 @@
     </row>
     <row r="4" spans="1:18">
       <c r="A4" s="51" t="str">
-        <f>DEC2HEX(0, 4)</f>
-        <v>0000</v>
+        <f>DEC2HEX(0, 8)</f>
+        <v>00000000</v>
       </c>
       <c r="C4" s="74" t="s">
         <v>60</v>
@@ -1907,8 +1981,8 @@
     </row>
     <row r="5" spans="1:18">
       <c r="A5" s="51" t="str">
-        <f>DEC2HEX(A4+16, 4)</f>
-        <v>0010</v>
+        <f>DEC2HEX(HEX2DEC(A4)+16, 8)</f>
+        <v>00000010</v>
       </c>
       <c r="C5" s="52" t="s">
         <v>59</v>
@@ -1931,8 +2005,8 @@
     </row>
     <row r="6" spans="1:18">
       <c r="A6" s="51" t="str">
-        <f>DEC2HEX(HEX2DEC(A5)+16, 4)</f>
-        <v>0020</v>
+        <f t="shared" ref="A6:A69" si="0">DEC2HEX(HEX2DEC(A5)+16, 8)</f>
+        <v>00000020</v>
       </c>
       <c r="C6" s="55"/>
       <c r="D6" s="56"/>
@@ -1953,8 +2027,8 @@
     </row>
     <row r="7" spans="1:18">
       <c r="A7" s="51" t="str">
-        <f t="shared" ref="A7:A35" si="0">DEC2HEX(HEX2DEC(A6)+16, 4)</f>
-        <v>0030</v>
+        <f t="shared" si="0"/>
+        <v>00000030</v>
       </c>
       <c r="C7" s="55"/>
       <c r="D7" s="56"/>
@@ -1976,7 +2050,7 @@
     <row r="8" spans="1:18">
       <c r="A8" s="51" t="str">
         <f t="shared" si="0"/>
-        <v>0040</v>
+        <v>00000040</v>
       </c>
       <c r="C8" s="55"/>
       <c r="D8" s="56"/>
@@ -1998,7 +2072,7 @@
     <row r="9" spans="1:18">
       <c r="A9" s="51" t="str">
         <f t="shared" si="0"/>
-        <v>0050</v>
+        <v>00000050</v>
       </c>
       <c r="C9" s="55"/>
       <c r="D9" s="56"/>
@@ -2020,7 +2094,7 @@
     <row r="10" spans="1:18">
       <c r="A10" s="51" t="str">
         <f t="shared" si="0"/>
-        <v>0060</v>
+        <v>00000060</v>
       </c>
       <c r="C10" s="55"/>
       <c r="D10" s="56"/>
@@ -2042,7 +2116,7 @@
     <row r="11" spans="1:18">
       <c r="A11" s="51" t="str">
         <f t="shared" si="0"/>
-        <v>0070</v>
+        <v>00000070</v>
       </c>
       <c r="C11" s="55"/>
       <c r="D11" s="56"/>
@@ -2064,7 +2138,7 @@
     <row r="12" spans="1:18">
       <c r="A12" s="51" t="str">
         <f t="shared" si="0"/>
-        <v>0080</v>
+        <v>00000080</v>
       </c>
       <c r="C12" s="55"/>
       <c r="D12" s="56"/>
@@ -2086,7 +2160,7 @@
     <row r="13" spans="1:18">
       <c r="A13" s="51" t="str">
         <f t="shared" si="0"/>
-        <v>0090</v>
+        <v>00000090</v>
       </c>
       <c r="C13" s="55"/>
       <c r="D13" s="56"/>
@@ -2108,7 +2182,7 @@
     <row r="14" spans="1:18">
       <c r="A14" s="51" t="str">
         <f t="shared" si="0"/>
-        <v>00A0</v>
+        <v>000000A0</v>
       </c>
       <c r="C14" s="55"/>
       <c r="D14" s="56"/>
@@ -2130,7 +2204,7 @@
     <row r="15" spans="1:18">
       <c r="A15" s="51" t="str">
         <f t="shared" si="0"/>
-        <v>00B0</v>
+        <v>000000B0</v>
       </c>
       <c r="C15" s="55"/>
       <c r="D15" s="56"/>
@@ -2152,7 +2226,7 @@
     <row r="16" spans="1:18">
       <c r="A16" s="51" t="str">
         <f t="shared" si="0"/>
-        <v>00C0</v>
+        <v>000000C0</v>
       </c>
       <c r="C16" s="55"/>
       <c r="D16" s="56"/>
@@ -2174,7 +2248,7 @@
     <row r="17" spans="1:18">
       <c r="A17" s="51" t="str">
         <f t="shared" si="0"/>
-        <v>00D0</v>
+        <v>000000D0</v>
       </c>
       <c r="C17" s="55"/>
       <c r="D17" s="56"/>
@@ -2196,7 +2270,7 @@
     <row r="18" spans="1:18">
       <c r="A18" s="51" t="str">
         <f t="shared" si="0"/>
-        <v>00E0</v>
+        <v>000000E0</v>
       </c>
       <c r="C18" s="55"/>
       <c r="D18" s="56"/>
@@ -2218,7 +2292,7 @@
     <row r="19" spans="1:18">
       <c r="A19" s="51" t="str">
         <f t="shared" si="0"/>
-        <v>00F0</v>
+        <v>000000F0</v>
       </c>
       <c r="C19" s="55"/>
       <c r="D19" s="56"/>
@@ -2240,7 +2314,7 @@
     <row r="20" spans="1:18">
       <c r="A20" s="51" t="str">
         <f t="shared" si="0"/>
-        <v>0100</v>
+        <v>00000100</v>
       </c>
       <c r="C20" s="58"/>
       <c r="D20" s="59"/>
@@ -2262,7 +2336,7 @@
     <row r="21" spans="1:18">
       <c r="A21" s="51" t="str">
         <f t="shared" si="0"/>
-        <v>0110</v>
+        <v>00000110</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
@@ -2284,7 +2358,7 @@
     <row r="22" spans="1:18">
       <c r="A22" s="51" t="str">
         <f t="shared" si="0"/>
-        <v>0120</v>
+        <v>00000120</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
@@ -2306,149 +2380,870 @@
     <row r="23" spans="1:18">
       <c r="A23" s="51" t="str">
         <f t="shared" si="0"/>
-        <v>0130</v>
-      </c>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
-      <c r="J23" s="2"/>
-      <c r="K23" s="2"/>
-      <c r="L23" s="2"/>
-      <c r="M23" s="2"/>
-      <c r="N23" s="2"/>
-      <c r="O23" s="2"/>
-      <c r="P23" s="2"/>
-      <c r="Q23" s="2"/>
-      <c r="R23" s="2"/>
+        <v>00000130</v>
+      </c>
+      <c r="C23" s="78" t="s">
+        <v>61</v>
+      </c>
+      <c r="D23" s="79"/>
+      <c r="E23" s="79"/>
+      <c r="F23" s="79"/>
+      <c r="G23" s="79"/>
+      <c r="H23" s="79"/>
+      <c r="I23" s="79"/>
+      <c r="J23" s="79"/>
+      <c r="K23" s="79"/>
+      <c r="L23" s="79"/>
+      <c r="M23" s="79"/>
+      <c r="N23" s="79"/>
+      <c r="O23" s="79"/>
+      <c r="P23" s="79"/>
+      <c r="Q23" s="79"/>
+      <c r="R23" s="80"/>
     </row>
     <row r="24" spans="1:18">
       <c r="A24" s="51" t="str">
         <f t="shared" si="0"/>
-        <v>0140</v>
-      </c>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-      <c r="I24" s="2"/>
-      <c r="J24" s="2"/>
-      <c r="K24" s="2"/>
-      <c r="L24" s="2"/>
-      <c r="M24" s="2"/>
-      <c r="N24" s="2"/>
-      <c r="O24" s="2"/>
-      <c r="P24" s="2"/>
-      <c r="Q24" s="2"/>
-      <c r="R24" s="2"/>
+        <v>00000140</v>
+      </c>
+      <c r="C24" s="78" t="s">
+        <v>62</v>
+      </c>
+      <c r="D24" s="79"/>
+      <c r="E24" s="79"/>
+      <c r="F24" s="79"/>
+      <c r="G24" s="79"/>
+      <c r="H24" s="79"/>
+      <c r="I24" s="79"/>
+      <c r="J24" s="79"/>
+      <c r="K24" s="79"/>
+      <c r="L24" s="79"/>
+      <c r="M24" s="79"/>
+      <c r="N24" s="79"/>
+      <c r="O24" s="79"/>
+      <c r="P24" s="79"/>
+      <c r="Q24" s="79"/>
+      <c r="R24" s="80"/>
     </row>
     <row r="25" spans="1:18">
       <c r="A25" s="51" t="str">
         <f t="shared" si="0"/>
-        <v>0150</v>
-      </c>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
-      <c r="I25" s="2"/>
-      <c r="J25" s="2"/>
-      <c r="K25" s="2"/>
-      <c r="L25" s="2"/>
-      <c r="M25" s="2"/>
-      <c r="N25" s="2"/>
-      <c r="O25" s="2"/>
-      <c r="P25" s="2"/>
-      <c r="Q25" s="2"/>
-      <c r="R25" s="2"/>
+        <v>00000150</v>
+      </c>
+      <c r="C25" s="78" t="s">
+        <v>63</v>
+      </c>
+      <c r="D25" s="79"/>
+      <c r="E25" s="79"/>
+      <c r="F25" s="79"/>
+      <c r="G25" s="79"/>
+      <c r="H25" s="79"/>
+      <c r="I25" s="79"/>
+      <c r="J25" s="79"/>
+      <c r="K25" s="79"/>
+      <c r="L25" s="79"/>
+      <c r="M25" s="79"/>
+      <c r="N25" s="79"/>
+      <c r="O25" s="79"/>
+      <c r="P25" s="79"/>
+      <c r="Q25" s="79"/>
+      <c r="R25" s="80"/>
     </row>
     <row r="26" spans="1:18">
       <c r="A26" s="51" t="str">
         <f t="shared" si="0"/>
-        <v>0160</v>
-      </c>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
-      <c r="I26" s="2"/>
-      <c r="J26" s="2"/>
-      <c r="K26" s="2"/>
-      <c r="L26" s="2"/>
-      <c r="M26" s="2"/>
-      <c r="N26" s="2"/>
-      <c r="O26" s="2"/>
-      <c r="P26" s="2"/>
-      <c r="Q26" s="2"/>
-      <c r="R26" s="2"/>
+        <v>00000160</v>
+      </c>
+      <c r="C26" s="78" t="s">
+        <v>64</v>
+      </c>
+      <c r="D26" s="79"/>
+      <c r="E26" s="79"/>
+      <c r="F26" s="79"/>
+      <c r="G26" s="79"/>
+      <c r="H26" s="79"/>
+      <c r="I26" s="79"/>
+      <c r="J26" s="79"/>
+      <c r="K26" s="79"/>
+      <c r="L26" s="79"/>
+      <c r="M26" s="79"/>
+      <c r="N26" s="79"/>
+      <c r="O26" s="79"/>
+      <c r="P26" s="79"/>
+      <c r="Q26" s="79"/>
+      <c r="R26" s="80"/>
     </row>
     <row r="27" spans="1:18">
       <c r="A27" s="51" t="str">
         <f t="shared" si="0"/>
-        <v>0170</v>
-      </c>
+        <v>00000170</v>
+      </c>
+      <c r="C27" s="78" t="s">
+        <v>65</v>
+      </c>
+      <c r="D27" s="79"/>
+      <c r="E27" s="79"/>
+      <c r="F27" s="79"/>
+      <c r="G27" s="79"/>
+      <c r="H27" s="79"/>
+      <c r="I27" s="79"/>
+      <c r="J27" s="79"/>
+      <c r="K27" s="79"/>
+      <c r="L27" s="79"/>
+      <c r="M27" s="79"/>
+      <c r="N27" s="79"/>
+      <c r="O27" s="79"/>
+      <c r="P27" s="79"/>
+      <c r="Q27" s="79"/>
+      <c r="R27" s="80"/>
     </row>
     <row r="28" spans="1:18">
       <c r="A28" s="51" t="str">
         <f t="shared" si="0"/>
-        <v>0180</v>
-      </c>
+        <v>00000180</v>
+      </c>
+      <c r="C28" s="78" t="s">
+        <v>66</v>
+      </c>
+      <c r="D28" s="79"/>
+      <c r="E28" s="79"/>
+      <c r="F28" s="79"/>
+      <c r="G28" s="79"/>
+      <c r="H28" s="79"/>
+      <c r="I28" s="79"/>
+      <c r="J28" s="79"/>
+      <c r="K28" s="79"/>
+      <c r="L28" s="79"/>
+      <c r="M28" s="79"/>
+      <c r="N28" s="79"/>
+      <c r="O28" s="79"/>
+      <c r="P28" s="79"/>
+      <c r="Q28" s="79"/>
+      <c r="R28" s="80"/>
     </row>
     <row r="29" spans="1:18">
       <c r="A29" s="51" t="str">
         <f t="shared" si="0"/>
-        <v>0190</v>
-      </c>
+        <v>00000190</v>
+      </c>
+      <c r="C29" s="78" t="s">
+        <v>67</v>
+      </c>
+      <c r="D29" s="79"/>
+      <c r="E29" s="79"/>
+      <c r="F29" s="79"/>
+      <c r="G29" s="79"/>
+      <c r="H29" s="79"/>
+      <c r="I29" s="79"/>
+      <c r="J29" s="79"/>
+      <c r="K29" s="79"/>
+      <c r="L29" s="79"/>
+      <c r="M29" s="79"/>
+      <c r="N29" s="79"/>
+      <c r="O29" s="79"/>
+      <c r="P29" s="79"/>
+      <c r="Q29" s="79"/>
+      <c r="R29" s="80"/>
     </row>
     <row r="30" spans="1:18">
       <c r="A30" s="51" t="str">
         <f t="shared" si="0"/>
-        <v>01A0</v>
-      </c>
+        <v>000001A0</v>
+      </c>
+      <c r="C30" s="78" t="s">
+        <v>68</v>
+      </c>
+      <c r="D30" s="79"/>
+      <c r="E30" s="79"/>
+      <c r="F30" s="79"/>
+      <c r="G30" s="79"/>
+      <c r="H30" s="79"/>
+      <c r="I30" s="79"/>
+      <c r="J30" s="79"/>
+      <c r="K30" s="79"/>
+      <c r="L30" s="79"/>
+      <c r="M30" s="79"/>
+      <c r="N30" s="79"/>
+      <c r="O30" s="79"/>
+      <c r="P30" s="79"/>
+      <c r="Q30" s="79"/>
+      <c r="R30" s="80"/>
     </row>
     <row r="31" spans="1:18">
       <c r="A31" s="51" t="str">
         <f t="shared" si="0"/>
-        <v>01B0</v>
-      </c>
+        <v>000001B0</v>
+      </c>
+      <c r="C31" s="78" t="s">
+        <v>69</v>
+      </c>
+      <c r="D31" s="79"/>
+      <c r="E31" s="79"/>
+      <c r="F31" s="79"/>
+      <c r="G31" s="79"/>
+      <c r="H31" s="79"/>
+      <c r="I31" s="79"/>
+      <c r="J31" s="79"/>
+      <c r="K31" s="79"/>
+      <c r="L31" s="79"/>
+      <c r="M31" s="79"/>
+      <c r="N31" s="79"/>
+      <c r="O31" s="79"/>
+      <c r="P31" s="79"/>
+      <c r="Q31" s="79"/>
+      <c r="R31" s="80"/>
     </row>
     <row r="32" spans="1:18">
       <c r="A32" s="51" t="str">
         <f t="shared" si="0"/>
-        <v>01C0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1">
+        <v>000001C0</v>
+      </c>
+      <c r="C32" s="78" t="s">
+        <v>70</v>
+      </c>
+      <c r="D32" s="79"/>
+      <c r="E32" s="79"/>
+      <c r="F32" s="79"/>
+      <c r="G32" s="79"/>
+      <c r="H32" s="79"/>
+      <c r="I32" s="79"/>
+      <c r="J32" s="79"/>
+      <c r="K32" s="79"/>
+      <c r="L32" s="79"/>
+      <c r="M32" s="79"/>
+      <c r="N32" s="79"/>
+      <c r="O32" s="79"/>
+      <c r="P32" s="79"/>
+      <c r="Q32" s="79"/>
+      <c r="R32" s="80"/>
+    </row>
+    <row r="33" spans="1:18">
       <c r="A33" s="51" t="str">
         <f t="shared" si="0"/>
-        <v>01D0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1">
+        <v>000001D0</v>
+      </c>
+      <c r="C33" s="78" t="s">
+        <v>71</v>
+      </c>
+      <c r="D33" s="79"/>
+      <c r="E33" s="79"/>
+      <c r="F33" s="79"/>
+      <c r="G33" s="79"/>
+      <c r="H33" s="79"/>
+      <c r="I33" s="79"/>
+      <c r="J33" s="79"/>
+      <c r="K33" s="79"/>
+      <c r="L33" s="79"/>
+      <c r="M33" s="79"/>
+      <c r="N33" s="79"/>
+      <c r="O33" s="79"/>
+      <c r="P33" s="79"/>
+      <c r="Q33" s="79"/>
+      <c r="R33" s="80"/>
+    </row>
+    <row r="34" spans="1:18">
       <c r="A34" s="51" t="str">
         <f t="shared" si="0"/>
-        <v>01E0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1">
+        <v>000001E0</v>
+      </c>
+      <c r="C34" s="78" t="s">
+        <v>72</v>
+      </c>
+      <c r="D34" s="79"/>
+      <c r="E34" s="79"/>
+      <c r="F34" s="79"/>
+      <c r="G34" s="79"/>
+      <c r="H34" s="79"/>
+      <c r="I34" s="79"/>
+      <c r="J34" s="79"/>
+      <c r="K34" s="79"/>
+      <c r="L34" s="79"/>
+      <c r="M34" s="79"/>
+      <c r="N34" s="79"/>
+      <c r="O34" s="79"/>
+      <c r="P34" s="79"/>
+      <c r="Q34" s="79"/>
+      <c r="R34" s="80"/>
+    </row>
+    <row r="35" spans="1:18">
       <c r="A35" s="51" t="str">
         <f t="shared" si="0"/>
-        <v>01F0</v>
+        <v>000001F0</v>
+      </c>
+      <c r="C35" s="78" t="s">
+        <v>73</v>
+      </c>
+      <c r="D35" s="79"/>
+      <c r="E35" s="79"/>
+      <c r="F35" s="79"/>
+      <c r="G35" s="79"/>
+      <c r="H35" s="79"/>
+      <c r="I35" s="79"/>
+      <c r="J35" s="79"/>
+      <c r="K35" s="79"/>
+      <c r="L35" s="79"/>
+      <c r="M35" s="79"/>
+      <c r="N35" s="79"/>
+      <c r="O35" s="79"/>
+      <c r="P35" s="79"/>
+      <c r="Q35" s="79"/>
+      <c r="R35" s="80"/>
+    </row>
+    <row r="36" spans="1:18">
+      <c r="A36" s="51" t="str">
+        <f t="shared" si="0"/>
+        <v>00000200</v>
+      </c>
+      <c r="C36" s="78" t="s">
+        <v>74</v>
+      </c>
+      <c r="D36" s="79"/>
+      <c r="E36" s="79"/>
+      <c r="F36" s="79"/>
+      <c r="G36" s="79"/>
+      <c r="H36" s="79"/>
+      <c r="I36" s="79"/>
+      <c r="J36" s="79"/>
+      <c r="K36" s="79"/>
+      <c r="L36" s="79"/>
+      <c r="M36" s="79"/>
+      <c r="N36" s="79"/>
+      <c r="O36" s="79"/>
+      <c r="P36" s="79"/>
+      <c r="Q36" s="79"/>
+      <c r="R36" s="80"/>
+    </row>
+    <row r="37" spans="1:18">
+      <c r="A37" s="51" t="str">
+        <f t="shared" si="0"/>
+        <v>00000210</v>
+      </c>
+      <c r="C37" s="78" t="s">
+        <v>75</v>
+      </c>
+      <c r="D37" s="79"/>
+      <c r="E37" s="79"/>
+      <c r="F37" s="79"/>
+      <c r="G37" s="79"/>
+      <c r="H37" s="79"/>
+      <c r="I37" s="79"/>
+      <c r="J37" s="79"/>
+      <c r="K37" s="79"/>
+      <c r="L37" s="79"/>
+      <c r="M37" s="79"/>
+      <c r="N37" s="79"/>
+      <c r="O37" s="79"/>
+      <c r="P37" s="79"/>
+      <c r="Q37" s="79"/>
+      <c r="R37" s="80"/>
+    </row>
+    <row r="38" spans="1:18">
+      <c r="A38" s="51" t="str">
+        <f t="shared" si="0"/>
+        <v>00000220</v>
+      </c>
+      <c r="C38" s="78" t="s">
+        <v>76</v>
+      </c>
+      <c r="D38" s="79"/>
+      <c r="E38" s="79"/>
+      <c r="F38" s="79"/>
+      <c r="G38" s="79"/>
+      <c r="H38" s="79"/>
+      <c r="I38" s="79"/>
+      <c r="J38" s="79"/>
+      <c r="K38" s="79"/>
+      <c r="L38" s="79"/>
+      <c r="M38" s="79"/>
+      <c r="N38" s="79"/>
+      <c r="O38" s="79"/>
+      <c r="P38" s="79"/>
+      <c r="Q38" s="79"/>
+      <c r="R38" s="80"/>
+    </row>
+    <row r="39" spans="1:18">
+      <c r="A39" s="51" t="str">
+        <f t="shared" si="0"/>
+        <v>00000230</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18">
+      <c r="A40" s="51" t="str">
+        <f t="shared" si="0"/>
+        <v>00000240</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18">
+      <c r="A41" s="51" t="str">
+        <f t="shared" si="0"/>
+        <v>00000250</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18">
+      <c r="A42" s="51" t="str">
+        <f t="shared" si="0"/>
+        <v>00000260</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18">
+      <c r="A43" s="51" t="str">
+        <f t="shared" si="0"/>
+        <v>00000270</v>
+      </c>
+    </row>
+    <row r="44" spans="1:18">
+      <c r="A44" s="51" t="str">
+        <f t="shared" si="0"/>
+        <v>00000280</v>
+      </c>
+    </row>
+    <row r="45" spans="1:18">
+      <c r="A45" s="51" t="str">
+        <f t="shared" si="0"/>
+        <v>00000290</v>
+      </c>
+    </row>
+    <row r="46" spans="1:18">
+      <c r="A46" s="51" t="str">
+        <f t="shared" si="0"/>
+        <v>000002A0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:18">
+      <c r="A47" s="51" t="str">
+        <f t="shared" si="0"/>
+        <v>000002B0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:18">
+      <c r="A48" s="51" t="str">
+        <f t="shared" si="0"/>
+        <v>000002C0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1">
+      <c r="A49" s="51" t="str">
+        <f t="shared" si="0"/>
+        <v>000002D0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1">
+      <c r="A50" s="51" t="str">
+        <f t="shared" si="0"/>
+        <v>000002E0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1">
+      <c r="A51" s="51" t="str">
+        <f t="shared" si="0"/>
+        <v>000002F0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1">
+      <c r="A52" s="51" t="str">
+        <f t="shared" si="0"/>
+        <v>00000300</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1">
+      <c r="A53" s="51" t="str">
+        <f t="shared" si="0"/>
+        <v>00000310</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1">
+      <c r="A54" s="51" t="str">
+        <f t="shared" si="0"/>
+        <v>00000320</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1">
+      <c r="A55" s="51" t="str">
+        <f t="shared" si="0"/>
+        <v>00000330</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1">
+      <c r="A56" s="51" t="str">
+        <f t="shared" si="0"/>
+        <v>00000340</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1">
+      <c r="A57" s="51" t="str">
+        <f t="shared" si="0"/>
+        <v>00000350</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1">
+      <c r="A58" s="51" t="str">
+        <f t="shared" si="0"/>
+        <v>00000360</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1">
+      <c r="A59" s="51" t="str">
+        <f t="shared" si="0"/>
+        <v>00000370</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1">
+      <c r="A60" s="51" t="str">
+        <f t="shared" si="0"/>
+        <v>00000380</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1">
+      <c r="A61" s="51" t="str">
+        <f t="shared" si="0"/>
+        <v>00000390</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1">
+      <c r="A62" s="51" t="str">
+        <f t="shared" si="0"/>
+        <v>000003A0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1">
+      <c r="A63" s="51" t="str">
+        <f t="shared" si="0"/>
+        <v>000003B0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1">
+      <c r="A64" s="51" t="str">
+        <f t="shared" si="0"/>
+        <v>000003C0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1">
+      <c r="A65" s="51" t="str">
+        <f t="shared" si="0"/>
+        <v>000003D0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1">
+      <c r="A66" s="51" t="str">
+        <f t="shared" si="0"/>
+        <v>000003E0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1">
+      <c r="A67" s="51" t="str">
+        <f t="shared" si="0"/>
+        <v>000003F0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1">
+      <c r="A68" s="51" t="str">
+        <f t="shared" si="0"/>
+        <v>00000400</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1">
+      <c r="A69" s="51" t="str">
+        <f t="shared" si="0"/>
+        <v>00000410</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1">
+      <c r="A70" s="51" t="str">
+        <f t="shared" ref="A70:A115" si="1">DEC2HEX(HEX2DEC(A69)+16, 8)</f>
+        <v>00000420</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1">
+      <c r="A71" s="51" t="str">
+        <f t="shared" si="1"/>
+        <v>00000430</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1">
+      <c r="A72" s="51" t="str">
+        <f t="shared" si="1"/>
+        <v>00000440</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1">
+      <c r="A73" s="51" t="str">
+        <f t="shared" si="1"/>
+        <v>00000450</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1">
+      <c r="A74" s="51" t="str">
+        <f t="shared" si="1"/>
+        <v>00000460</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1">
+      <c r="A75" s="51" t="str">
+        <f t="shared" si="1"/>
+        <v>00000470</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1">
+      <c r="A76" s="51" t="str">
+        <f t="shared" si="1"/>
+        <v>00000480</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1">
+      <c r="A77" s="51" t="str">
+        <f t="shared" si="1"/>
+        <v>00000490</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1">
+      <c r="A78" s="51" t="str">
+        <f t="shared" si="1"/>
+        <v>000004A0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1">
+      <c r="A79" s="51" t="str">
+        <f t="shared" si="1"/>
+        <v>000004B0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1">
+      <c r="A80" s="51" t="str">
+        <f t="shared" si="1"/>
+        <v>000004C0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1">
+      <c r="A81" s="51" t="str">
+        <f t="shared" si="1"/>
+        <v>000004D0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1">
+      <c r="A82" s="51" t="str">
+        <f t="shared" si="1"/>
+        <v>000004E0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1">
+      <c r="A83" s="51" t="str">
+        <f t="shared" si="1"/>
+        <v>000004F0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1">
+      <c r="A84" s="51" t="str">
+        <f t="shared" si="1"/>
+        <v>00000500</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1">
+      <c r="A85" s="51" t="str">
+        <f t="shared" si="1"/>
+        <v>00000510</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1">
+      <c r="A86" s="51" t="str">
+        <f t="shared" si="1"/>
+        <v>00000520</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1">
+      <c r="A87" s="51" t="str">
+        <f t="shared" si="1"/>
+        <v>00000530</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1">
+      <c r="A88" s="51" t="str">
+        <f t="shared" si="1"/>
+        <v>00000540</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1">
+      <c r="A89" s="51" t="str">
+        <f t="shared" si="1"/>
+        <v>00000550</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1">
+      <c r="A90" s="51" t="str">
+        <f t="shared" si="1"/>
+        <v>00000560</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1">
+      <c r="A91" s="51" t="str">
+        <f t="shared" si="1"/>
+        <v>00000570</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1">
+      <c r="A92" s="51" t="str">
+        <f t="shared" si="1"/>
+        <v>00000580</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1">
+      <c r="A93" s="51" t="str">
+        <f t="shared" si="1"/>
+        <v>00000590</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1">
+      <c r="A94" s="51" t="str">
+        <f t="shared" si="1"/>
+        <v>000005A0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1">
+      <c r="A95" s="51" t="str">
+        <f t="shared" si="1"/>
+        <v>000005B0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1">
+      <c r="A96" s="51" t="str">
+        <f t="shared" si="1"/>
+        <v>000005C0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1">
+      <c r="A97" s="51" t="str">
+        <f t="shared" si="1"/>
+        <v>000005D0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1">
+      <c r="A98" s="51" t="str">
+        <f t="shared" si="1"/>
+        <v>000005E0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1">
+      <c r="A99" s="51" t="str">
+        <f t="shared" si="1"/>
+        <v>000005F0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1">
+      <c r="A100" s="51" t="str">
+        <f t="shared" si="1"/>
+        <v>00000600</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1">
+      <c r="A101" s="51" t="str">
+        <f t="shared" si="1"/>
+        <v>00000610</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1">
+      <c r="A102" s="51" t="str">
+        <f t="shared" si="1"/>
+        <v>00000620</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1">
+      <c r="A103" s="51" t="str">
+        <f t="shared" si="1"/>
+        <v>00000630</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1">
+      <c r="A104" s="51" t="str">
+        <f t="shared" si="1"/>
+        <v>00000640</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1">
+      <c r="A105" s="51" t="str">
+        <f t="shared" si="1"/>
+        <v>00000650</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1">
+      <c r="A106" s="51" t="str">
+        <f t="shared" si="1"/>
+        <v>00000660</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1">
+      <c r="A107" s="51" t="str">
+        <f t="shared" si="1"/>
+        <v>00000670</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1">
+      <c r="A108" s="51" t="str">
+        <f t="shared" si="1"/>
+        <v>00000680</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1">
+      <c r="A109" s="51" t="str">
+        <f t="shared" si="1"/>
+        <v>00000690</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1">
+      <c r="A110" s="51" t="str">
+        <f t="shared" si="1"/>
+        <v>000006A0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1">
+      <c r="A111" s="51" t="str">
+        <f t="shared" si="1"/>
+        <v>000006B0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1">
+      <c r="A112" s="51" t="str">
+        <f t="shared" si="1"/>
+        <v>000006C0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1">
+      <c r="A113" s="51" t="str">
+        <f t="shared" si="1"/>
+        <v>000006D0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1">
+      <c r="A114" s="51" t="str">
+        <f t="shared" si="1"/>
+        <v>000006E0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1">
+      <c r="A115" s="51" t="str">
+        <f t="shared" si="1"/>
+        <v>000006F0</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="19">
+    <mergeCell ref="C38:R38"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="C32:R32"/>
+    <mergeCell ref="C33:R33"/>
+    <mergeCell ref="C34:R34"/>
+    <mergeCell ref="C35:R35"/>
+    <mergeCell ref="C36:R36"/>
+    <mergeCell ref="C37:R37"/>
+    <mergeCell ref="C26:R26"/>
+    <mergeCell ref="C27:R27"/>
+    <mergeCell ref="C28:R28"/>
+    <mergeCell ref="C29:R29"/>
+    <mergeCell ref="C30:R30"/>
+    <mergeCell ref="C31:R31"/>
     <mergeCell ref="G4:J4"/>
     <mergeCell ref="C5:R20"/>
+    <mergeCell ref="C23:R23"/>
+    <mergeCell ref="C24:R24"/>
+    <mergeCell ref="C25:R25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2459,7 +3254,7 @@
   <dimension ref="A1:R30"/>
   <sheetViews>
     <sheetView showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13:F13"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>

</xml_diff>

<commit_message>
Include new motor interface
</commit_message>
<xml_diff>
--- a/docs/Memory_Sheet.xlsx
+++ b/docs/Memory_Sheet.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="16560" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="16560" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Private Block" sheetId="4" r:id="rId1"/>
@@ -44,9 +44,6 @@
     <t>TYPE</t>
   </si>
   <si>
-    <t>CONTROL PERIOD</t>
-  </si>
-  <si>
     <t>SRX Extended Block</t>
   </si>
   <si>
@@ -264,6 +261,9 @@
   </si>
   <si>
     <t>SPEED CONTROLLER / MOTOR</t>
+  </si>
+  <si>
+    <t>BOOTSTRAP_INIT</t>
   </si>
 </sst>
 </file>
@@ -551,7 +551,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -749,6 +749,9 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1089,7 +1092,7 @@
     <row r="1" spans="1:18" ht="9.9499999999999993" customHeight="1"/>
     <row r="2" spans="1:18">
       <c r="C2" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:18">
@@ -1124,22 +1127,22 @@
         <v>9</v>
       </c>
       <c r="M3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="N3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N3" s="3" t="s">
+      <c r="O3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O3" s="3" t="s">
+      <c r="P3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P3" s="3" t="s">
+      <c r="Q3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="Q3" s="3" t="s">
+      <c r="R3" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="R3" s="3" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:18">
@@ -1147,17 +1150,17 @@
         <f>DEC2HEX(0, 4)</f>
         <v>0000</v>
       </c>
-      <c r="C4" s="74" t="s">
-        <v>60</v>
+      <c r="C4" s="75" t="s">
+        <v>59</v>
       </c>
       <c r="D4" s="47" t="s">
+        <v>46</v>
+      </c>
+      <c r="E4" s="74" t="s">
         <v>47</v>
       </c>
-      <c r="E4" s="73" t="s">
+      <c r="F4" s="47" t="s">
         <v>48</v>
-      </c>
-      <c r="F4" s="47" t="s">
-        <v>49</v>
       </c>
       <c r="G4" s="48"/>
       <c r="H4" s="48"/>
@@ -1178,7 +1181,7 @@
         <v>0010</v>
       </c>
       <c r="C5" s="52" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D5" s="53"/>
       <c r="E5" s="53"/>
@@ -1510,7 +1513,7 @@
         <v>0100</v>
       </c>
       <c r="C20" s="61" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D20" s="62"/>
       <c r="E20" s="62"/>
@@ -1872,8 +1875,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R115"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+    <sheetView showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -1890,13 +1893,13 @@
     <row r="1" spans="1:18" ht="9.9499999999999993" customHeight="1"/>
     <row r="2" spans="1:18">
       <c r="C2" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="F2" s="75" t="s">
-        <v>77</v>
-      </c>
-      <c r="G2" s="76"/>
-      <c r="H2" s="77"/>
+        <v>49</v>
+      </c>
+      <c r="F2" s="76" t="s">
+        <v>76</v>
+      </c>
+      <c r="G2" s="77"/>
+      <c r="H2" s="78"/>
     </row>
     <row r="3" spans="1:18">
       <c r="C3" s="3">
@@ -1930,22 +1933,22 @@
         <v>9</v>
       </c>
       <c r="M3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="N3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N3" s="3" t="s">
+      <c r="O3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O3" s="3" t="s">
+      <c r="P3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P3" s="3" t="s">
+      <c r="Q3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="Q3" s="3" t="s">
+      <c r="R3" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="R3" s="3" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:18">
@@ -1953,26 +1956,26 @@
         <f>DEC2HEX(0, 8)</f>
         <v>00000000</v>
       </c>
-      <c r="C4" s="74" t="s">
-        <v>60</v>
-      </c>
-      <c r="G4" s="70" t="s">
+      <c r="C4" s="75" t="s">
+        <v>59</v>
+      </c>
+      <c r="G4" s="71" t="s">
+        <v>51</v>
+      </c>
+      <c r="H4" s="72"/>
+      <c r="I4" s="72"/>
+      <c r="J4" s="73"/>
+      <c r="K4" s="74" t="s">
+        <v>53</v>
+      </c>
+      <c r="L4" s="74" t="s">
+        <v>54</v>
+      </c>
+      <c r="M4" s="74" t="s">
+        <v>57</v>
+      </c>
+      <c r="N4" s="74" t="s">
         <v>52</v>
-      </c>
-      <c r="H4" s="71"/>
-      <c r="I4" s="71"/>
-      <c r="J4" s="72"/>
-      <c r="K4" s="73" t="s">
-        <v>54</v>
-      </c>
-      <c r="L4" s="73" t="s">
-        <v>55</v>
-      </c>
-      <c r="M4" s="73" t="s">
-        <v>58</v>
-      </c>
-      <c r="N4" s="73" t="s">
-        <v>53</v>
       </c>
       <c r="O4" s="48"/>
       <c r="P4" s="48"/>
@@ -1985,7 +1988,7 @@
         <v>00000010</v>
       </c>
       <c r="C5" s="52" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D5" s="53"/>
       <c r="E5" s="53"/>
@@ -2382,384 +2385,384 @@
         <f t="shared" si="0"/>
         <v>00000130</v>
       </c>
-      <c r="C23" s="78" t="s">
-        <v>61</v>
-      </c>
-      <c r="D23" s="79"/>
-      <c r="E23" s="79"/>
-      <c r="F23" s="79"/>
-      <c r="G23" s="79"/>
-      <c r="H23" s="79"/>
-      <c r="I23" s="79"/>
-      <c r="J23" s="79"/>
-      <c r="K23" s="79"/>
-      <c r="L23" s="79"/>
-      <c r="M23" s="79"/>
-      <c r="N23" s="79"/>
-      <c r="O23" s="79"/>
-      <c r="P23" s="79"/>
-      <c r="Q23" s="79"/>
-      <c r="R23" s="80"/>
+      <c r="C23" s="79" t="s">
+        <v>60</v>
+      </c>
+      <c r="D23" s="80"/>
+      <c r="E23" s="80"/>
+      <c r="F23" s="80"/>
+      <c r="G23" s="80"/>
+      <c r="H23" s="80"/>
+      <c r="I23" s="80"/>
+      <c r="J23" s="80"/>
+      <c r="K23" s="80"/>
+      <c r="L23" s="80"/>
+      <c r="M23" s="80"/>
+      <c r="N23" s="80"/>
+      <c r="O23" s="80"/>
+      <c r="P23" s="80"/>
+      <c r="Q23" s="80"/>
+      <c r="R23" s="81"/>
     </row>
     <row r="24" spans="1:18">
       <c r="A24" s="51" t="str">
         <f t="shared" si="0"/>
         <v>00000140</v>
       </c>
-      <c r="C24" s="78" t="s">
-        <v>62</v>
-      </c>
-      <c r="D24" s="79"/>
-      <c r="E24" s="79"/>
-      <c r="F24" s="79"/>
-      <c r="G24" s="79"/>
-      <c r="H24" s="79"/>
-      <c r="I24" s="79"/>
-      <c r="J24" s="79"/>
-      <c r="K24" s="79"/>
-      <c r="L24" s="79"/>
-      <c r="M24" s="79"/>
-      <c r="N24" s="79"/>
-      <c r="O24" s="79"/>
-      <c r="P24" s="79"/>
-      <c r="Q24" s="79"/>
-      <c r="R24" s="80"/>
+      <c r="C24" s="79" t="s">
+        <v>61</v>
+      </c>
+      <c r="D24" s="80"/>
+      <c r="E24" s="80"/>
+      <c r="F24" s="80"/>
+      <c r="G24" s="80"/>
+      <c r="H24" s="80"/>
+      <c r="I24" s="80"/>
+      <c r="J24" s="80"/>
+      <c r="K24" s="80"/>
+      <c r="L24" s="80"/>
+      <c r="M24" s="80"/>
+      <c r="N24" s="80"/>
+      <c r="O24" s="80"/>
+      <c r="P24" s="80"/>
+      <c r="Q24" s="80"/>
+      <c r="R24" s="81"/>
     </row>
     <row r="25" spans="1:18">
       <c r="A25" s="51" t="str">
         <f t="shared" si="0"/>
         <v>00000150</v>
       </c>
-      <c r="C25" s="78" t="s">
-        <v>63</v>
-      </c>
-      <c r="D25" s="79"/>
-      <c r="E25" s="79"/>
-      <c r="F25" s="79"/>
-      <c r="G25" s="79"/>
-      <c r="H25" s="79"/>
-      <c r="I25" s="79"/>
-      <c r="J25" s="79"/>
-      <c r="K25" s="79"/>
-      <c r="L25" s="79"/>
-      <c r="M25" s="79"/>
-      <c r="N25" s="79"/>
-      <c r="O25" s="79"/>
-      <c r="P25" s="79"/>
-      <c r="Q25" s="79"/>
-      <c r="R25" s="80"/>
+      <c r="C25" s="79" t="s">
+        <v>62</v>
+      </c>
+      <c r="D25" s="80"/>
+      <c r="E25" s="80"/>
+      <c r="F25" s="80"/>
+      <c r="G25" s="80"/>
+      <c r="H25" s="80"/>
+      <c r="I25" s="80"/>
+      <c r="J25" s="80"/>
+      <c r="K25" s="80"/>
+      <c r="L25" s="80"/>
+      <c r="M25" s="80"/>
+      <c r="N25" s="80"/>
+      <c r="O25" s="80"/>
+      <c r="P25" s="80"/>
+      <c r="Q25" s="80"/>
+      <c r="R25" s="81"/>
     </row>
     <row r="26" spans="1:18">
       <c r="A26" s="51" t="str">
         <f t="shared" si="0"/>
         <v>00000160</v>
       </c>
-      <c r="C26" s="78" t="s">
-        <v>64</v>
-      </c>
-      <c r="D26" s="79"/>
-      <c r="E26" s="79"/>
-      <c r="F26" s="79"/>
-      <c r="G26" s="79"/>
-      <c r="H26" s="79"/>
-      <c r="I26" s="79"/>
-      <c r="J26" s="79"/>
-      <c r="K26" s="79"/>
-      <c r="L26" s="79"/>
-      <c r="M26" s="79"/>
-      <c r="N26" s="79"/>
-      <c r="O26" s="79"/>
-      <c r="P26" s="79"/>
-      <c r="Q26" s="79"/>
-      <c r="R26" s="80"/>
+      <c r="C26" s="79" t="s">
+        <v>63</v>
+      </c>
+      <c r="D26" s="80"/>
+      <c r="E26" s="80"/>
+      <c r="F26" s="80"/>
+      <c r="G26" s="80"/>
+      <c r="H26" s="80"/>
+      <c r="I26" s="80"/>
+      <c r="J26" s="80"/>
+      <c r="K26" s="80"/>
+      <c r="L26" s="80"/>
+      <c r="M26" s="80"/>
+      <c r="N26" s="80"/>
+      <c r="O26" s="80"/>
+      <c r="P26" s="80"/>
+      <c r="Q26" s="80"/>
+      <c r="R26" s="81"/>
     </row>
     <row r="27" spans="1:18">
       <c r="A27" s="51" t="str">
         <f t="shared" si="0"/>
         <v>00000170</v>
       </c>
-      <c r="C27" s="78" t="s">
-        <v>65</v>
-      </c>
-      <c r="D27" s="79"/>
-      <c r="E27" s="79"/>
-      <c r="F27" s="79"/>
-      <c r="G27" s="79"/>
-      <c r="H27" s="79"/>
-      <c r="I27" s="79"/>
-      <c r="J27" s="79"/>
-      <c r="K27" s="79"/>
-      <c r="L27" s="79"/>
-      <c r="M27" s="79"/>
-      <c r="N27" s="79"/>
-      <c r="O27" s="79"/>
-      <c r="P27" s="79"/>
-      <c r="Q27" s="79"/>
-      <c r="R27" s="80"/>
+      <c r="C27" s="79" t="s">
+        <v>64</v>
+      </c>
+      <c r="D27" s="80"/>
+      <c r="E27" s="80"/>
+      <c r="F27" s="80"/>
+      <c r="G27" s="80"/>
+      <c r="H27" s="80"/>
+      <c r="I27" s="80"/>
+      <c r="J27" s="80"/>
+      <c r="K27" s="80"/>
+      <c r="L27" s="80"/>
+      <c r="M27" s="80"/>
+      <c r="N27" s="80"/>
+      <c r="O27" s="80"/>
+      <c r="P27" s="80"/>
+      <c r="Q27" s="80"/>
+      <c r="R27" s="81"/>
     </row>
     <row r="28" spans="1:18">
       <c r="A28" s="51" t="str">
         <f t="shared" si="0"/>
         <v>00000180</v>
       </c>
-      <c r="C28" s="78" t="s">
-        <v>66</v>
-      </c>
-      <c r="D28" s="79"/>
-      <c r="E28" s="79"/>
-      <c r="F28" s="79"/>
-      <c r="G28" s="79"/>
-      <c r="H28" s="79"/>
-      <c r="I28" s="79"/>
-      <c r="J28" s="79"/>
-      <c r="K28" s="79"/>
-      <c r="L28" s="79"/>
-      <c r="M28" s="79"/>
-      <c r="N28" s="79"/>
-      <c r="O28" s="79"/>
-      <c r="P28" s="79"/>
-      <c r="Q28" s="79"/>
-      <c r="R28" s="80"/>
+      <c r="C28" s="79" t="s">
+        <v>65</v>
+      </c>
+      <c r="D28" s="80"/>
+      <c r="E28" s="80"/>
+      <c r="F28" s="80"/>
+      <c r="G28" s="80"/>
+      <c r="H28" s="80"/>
+      <c r="I28" s="80"/>
+      <c r="J28" s="80"/>
+      <c r="K28" s="80"/>
+      <c r="L28" s="80"/>
+      <c r="M28" s="80"/>
+      <c r="N28" s="80"/>
+      <c r="O28" s="80"/>
+      <c r="P28" s="80"/>
+      <c r="Q28" s="80"/>
+      <c r="R28" s="81"/>
     </row>
     <row r="29" spans="1:18">
       <c r="A29" s="51" t="str">
         <f t="shared" si="0"/>
         <v>00000190</v>
       </c>
-      <c r="C29" s="78" t="s">
-        <v>67</v>
-      </c>
-      <c r="D29" s="79"/>
-      <c r="E29" s="79"/>
-      <c r="F29" s="79"/>
-      <c r="G29" s="79"/>
-      <c r="H29" s="79"/>
-      <c r="I29" s="79"/>
-      <c r="J29" s="79"/>
-      <c r="K29" s="79"/>
-      <c r="L29" s="79"/>
-      <c r="M29" s="79"/>
-      <c r="N29" s="79"/>
-      <c r="O29" s="79"/>
-      <c r="P29" s="79"/>
-      <c r="Q29" s="79"/>
-      <c r="R29" s="80"/>
+      <c r="C29" s="79" t="s">
+        <v>66</v>
+      </c>
+      <c r="D29" s="80"/>
+      <c r="E29" s="80"/>
+      <c r="F29" s="80"/>
+      <c r="G29" s="80"/>
+      <c r="H29" s="80"/>
+      <c r="I29" s="80"/>
+      <c r="J29" s="80"/>
+      <c r="K29" s="80"/>
+      <c r="L29" s="80"/>
+      <c r="M29" s="80"/>
+      <c r="N29" s="80"/>
+      <c r="O29" s="80"/>
+      <c r="P29" s="80"/>
+      <c r="Q29" s="80"/>
+      <c r="R29" s="81"/>
     </row>
     <row r="30" spans="1:18">
       <c r="A30" s="51" t="str">
         <f t="shared" si="0"/>
         <v>000001A0</v>
       </c>
-      <c r="C30" s="78" t="s">
-        <v>68</v>
-      </c>
-      <c r="D30" s="79"/>
-      <c r="E30" s="79"/>
-      <c r="F30" s="79"/>
-      <c r="G30" s="79"/>
-      <c r="H30" s="79"/>
-      <c r="I30" s="79"/>
-      <c r="J30" s="79"/>
-      <c r="K30" s="79"/>
-      <c r="L30" s="79"/>
-      <c r="M30" s="79"/>
-      <c r="N30" s="79"/>
-      <c r="O30" s="79"/>
-      <c r="P30" s="79"/>
-      <c r="Q30" s="79"/>
-      <c r="R30" s="80"/>
+      <c r="C30" s="79" t="s">
+        <v>67</v>
+      </c>
+      <c r="D30" s="80"/>
+      <c r="E30" s="80"/>
+      <c r="F30" s="80"/>
+      <c r="G30" s="80"/>
+      <c r="H30" s="80"/>
+      <c r="I30" s="80"/>
+      <c r="J30" s="80"/>
+      <c r="K30" s="80"/>
+      <c r="L30" s="80"/>
+      <c r="M30" s="80"/>
+      <c r="N30" s="80"/>
+      <c r="O30" s="80"/>
+      <c r="P30" s="80"/>
+      <c r="Q30" s="80"/>
+      <c r="R30" s="81"/>
     </row>
     <row r="31" spans="1:18">
       <c r="A31" s="51" t="str">
         <f t="shared" si="0"/>
         <v>000001B0</v>
       </c>
-      <c r="C31" s="78" t="s">
-        <v>69</v>
-      </c>
-      <c r="D31" s="79"/>
-      <c r="E31" s="79"/>
-      <c r="F31" s="79"/>
-      <c r="G31" s="79"/>
-      <c r="H31" s="79"/>
-      <c r="I31" s="79"/>
-      <c r="J31" s="79"/>
-      <c r="K31" s="79"/>
-      <c r="L31" s="79"/>
-      <c r="M31" s="79"/>
-      <c r="N31" s="79"/>
-      <c r="O31" s="79"/>
-      <c r="P31" s="79"/>
-      <c r="Q31" s="79"/>
-      <c r="R31" s="80"/>
+      <c r="C31" s="79" t="s">
+        <v>68</v>
+      </c>
+      <c r="D31" s="80"/>
+      <c r="E31" s="80"/>
+      <c r="F31" s="80"/>
+      <c r="G31" s="80"/>
+      <c r="H31" s="80"/>
+      <c r="I31" s="80"/>
+      <c r="J31" s="80"/>
+      <c r="K31" s="80"/>
+      <c r="L31" s="80"/>
+      <c r="M31" s="80"/>
+      <c r="N31" s="80"/>
+      <c r="O31" s="80"/>
+      <c r="P31" s="80"/>
+      <c r="Q31" s="80"/>
+      <c r="R31" s="81"/>
     </row>
     <row r="32" spans="1:18">
       <c r="A32" s="51" t="str">
         <f t="shared" si="0"/>
         <v>000001C0</v>
       </c>
-      <c r="C32" s="78" t="s">
-        <v>70</v>
-      </c>
-      <c r="D32" s="79"/>
-      <c r="E32" s="79"/>
-      <c r="F32" s="79"/>
-      <c r="G32" s="79"/>
-      <c r="H32" s="79"/>
-      <c r="I32" s="79"/>
-      <c r="J32" s="79"/>
-      <c r="K32" s="79"/>
-      <c r="L32" s="79"/>
-      <c r="M32" s="79"/>
-      <c r="N32" s="79"/>
-      <c r="O32" s="79"/>
-      <c r="P32" s="79"/>
-      <c r="Q32" s="79"/>
-      <c r="R32" s="80"/>
+      <c r="C32" s="79" t="s">
+        <v>69</v>
+      </c>
+      <c r="D32" s="80"/>
+      <c r="E32" s="80"/>
+      <c r="F32" s="80"/>
+      <c r="G32" s="80"/>
+      <c r="H32" s="80"/>
+      <c r="I32" s="80"/>
+      <c r="J32" s="80"/>
+      <c r="K32" s="80"/>
+      <c r="L32" s="80"/>
+      <c r="M32" s="80"/>
+      <c r="N32" s="80"/>
+      <c r="O32" s="80"/>
+      <c r="P32" s="80"/>
+      <c r="Q32" s="80"/>
+      <c r="R32" s="81"/>
     </row>
     <row r="33" spans="1:18">
       <c r="A33" s="51" t="str">
         <f t="shared" si="0"/>
         <v>000001D0</v>
       </c>
-      <c r="C33" s="78" t="s">
-        <v>71</v>
-      </c>
-      <c r="D33" s="79"/>
-      <c r="E33" s="79"/>
-      <c r="F33" s="79"/>
-      <c r="G33" s="79"/>
-      <c r="H33" s="79"/>
-      <c r="I33" s="79"/>
-      <c r="J33" s="79"/>
-      <c r="K33" s="79"/>
-      <c r="L33" s="79"/>
-      <c r="M33" s="79"/>
-      <c r="N33" s="79"/>
-      <c r="O33" s="79"/>
-      <c r="P33" s="79"/>
-      <c r="Q33" s="79"/>
-      <c r="R33" s="80"/>
+      <c r="C33" s="79" t="s">
+        <v>70</v>
+      </c>
+      <c r="D33" s="80"/>
+      <c r="E33" s="80"/>
+      <c r="F33" s="80"/>
+      <c r="G33" s="80"/>
+      <c r="H33" s="80"/>
+      <c r="I33" s="80"/>
+      <c r="J33" s="80"/>
+      <c r="K33" s="80"/>
+      <c r="L33" s="80"/>
+      <c r="M33" s="80"/>
+      <c r="N33" s="80"/>
+      <c r="O33" s="80"/>
+      <c r="P33" s="80"/>
+      <c r="Q33" s="80"/>
+      <c r="R33" s="81"/>
     </row>
     <row r="34" spans="1:18">
       <c r="A34" s="51" t="str">
         <f t="shared" si="0"/>
         <v>000001E0</v>
       </c>
-      <c r="C34" s="78" t="s">
-        <v>72</v>
-      </c>
-      <c r="D34" s="79"/>
-      <c r="E34" s="79"/>
-      <c r="F34" s="79"/>
-      <c r="G34" s="79"/>
-      <c r="H34" s="79"/>
-      <c r="I34" s="79"/>
-      <c r="J34" s="79"/>
-      <c r="K34" s="79"/>
-      <c r="L34" s="79"/>
-      <c r="M34" s="79"/>
-      <c r="N34" s="79"/>
-      <c r="O34" s="79"/>
-      <c r="P34" s="79"/>
-      <c r="Q34" s="79"/>
-      <c r="R34" s="80"/>
+      <c r="C34" s="79" t="s">
+        <v>71</v>
+      </c>
+      <c r="D34" s="80"/>
+      <c r="E34" s="80"/>
+      <c r="F34" s="80"/>
+      <c r="G34" s="80"/>
+      <c r="H34" s="80"/>
+      <c r="I34" s="80"/>
+      <c r="J34" s="80"/>
+      <c r="K34" s="80"/>
+      <c r="L34" s="80"/>
+      <c r="M34" s="80"/>
+      <c r="N34" s="80"/>
+      <c r="O34" s="80"/>
+      <c r="P34" s="80"/>
+      <c r="Q34" s="80"/>
+      <c r="R34" s="81"/>
     </row>
     <row r="35" spans="1:18">
       <c r="A35" s="51" t="str">
         <f t="shared" si="0"/>
         <v>000001F0</v>
       </c>
-      <c r="C35" s="78" t="s">
-        <v>73</v>
-      </c>
-      <c r="D35" s="79"/>
-      <c r="E35" s="79"/>
-      <c r="F35" s="79"/>
-      <c r="G35" s="79"/>
-      <c r="H35" s="79"/>
-      <c r="I35" s="79"/>
-      <c r="J35" s="79"/>
-      <c r="K35" s="79"/>
-      <c r="L35" s="79"/>
-      <c r="M35" s="79"/>
-      <c r="N35" s="79"/>
-      <c r="O35" s="79"/>
-      <c r="P35" s="79"/>
-      <c r="Q35" s="79"/>
-      <c r="R35" s="80"/>
+      <c r="C35" s="79" t="s">
+        <v>72</v>
+      </c>
+      <c r="D35" s="80"/>
+      <c r="E35" s="80"/>
+      <c r="F35" s="80"/>
+      <c r="G35" s="80"/>
+      <c r="H35" s="80"/>
+      <c r="I35" s="80"/>
+      <c r="J35" s="80"/>
+      <c r="K35" s="80"/>
+      <c r="L35" s="80"/>
+      <c r="M35" s="80"/>
+      <c r="N35" s="80"/>
+      <c r="O35" s="80"/>
+      <c r="P35" s="80"/>
+      <c r="Q35" s="80"/>
+      <c r="R35" s="81"/>
     </row>
     <row r="36" spans="1:18">
       <c r="A36" s="51" t="str">
         <f t="shared" si="0"/>
         <v>00000200</v>
       </c>
-      <c r="C36" s="78" t="s">
-        <v>74</v>
-      </c>
-      <c r="D36" s="79"/>
-      <c r="E36" s="79"/>
-      <c r="F36" s="79"/>
-      <c r="G36" s="79"/>
-      <c r="H36" s="79"/>
-      <c r="I36" s="79"/>
-      <c r="J36" s="79"/>
-      <c r="K36" s="79"/>
-      <c r="L36" s="79"/>
-      <c r="M36" s="79"/>
-      <c r="N36" s="79"/>
-      <c r="O36" s="79"/>
-      <c r="P36" s="79"/>
-      <c r="Q36" s="79"/>
-      <c r="R36" s="80"/>
+      <c r="C36" s="79" t="s">
+        <v>73</v>
+      </c>
+      <c r="D36" s="80"/>
+      <c r="E36" s="80"/>
+      <c r="F36" s="80"/>
+      <c r="G36" s="80"/>
+      <c r="H36" s="80"/>
+      <c r="I36" s="80"/>
+      <c r="J36" s="80"/>
+      <c r="K36" s="80"/>
+      <c r="L36" s="80"/>
+      <c r="M36" s="80"/>
+      <c r="N36" s="80"/>
+      <c r="O36" s="80"/>
+      <c r="P36" s="80"/>
+      <c r="Q36" s="80"/>
+      <c r="R36" s="81"/>
     </row>
     <row r="37" spans="1:18">
       <c r="A37" s="51" t="str">
         <f t="shared" si="0"/>
         <v>00000210</v>
       </c>
-      <c r="C37" s="78" t="s">
-        <v>75</v>
-      </c>
-      <c r="D37" s="79"/>
-      <c r="E37" s="79"/>
-      <c r="F37" s="79"/>
-      <c r="G37" s="79"/>
-      <c r="H37" s="79"/>
-      <c r="I37" s="79"/>
-      <c r="J37" s="79"/>
-      <c r="K37" s="79"/>
-      <c r="L37" s="79"/>
-      <c r="M37" s="79"/>
-      <c r="N37" s="79"/>
-      <c r="O37" s="79"/>
-      <c r="P37" s="79"/>
-      <c r="Q37" s="79"/>
-      <c r="R37" s="80"/>
+      <c r="C37" s="79" t="s">
+        <v>74</v>
+      </c>
+      <c r="D37" s="80"/>
+      <c r="E37" s="80"/>
+      <c r="F37" s="80"/>
+      <c r="G37" s="80"/>
+      <c r="H37" s="80"/>
+      <c r="I37" s="80"/>
+      <c r="J37" s="80"/>
+      <c r="K37" s="80"/>
+      <c r="L37" s="80"/>
+      <c r="M37" s="80"/>
+      <c r="N37" s="80"/>
+      <c r="O37" s="80"/>
+      <c r="P37" s="80"/>
+      <c r="Q37" s="80"/>
+      <c r="R37" s="81"/>
     </row>
     <row r="38" spans="1:18">
       <c r="A38" s="51" t="str">
         <f t="shared" si="0"/>
         <v>00000220</v>
       </c>
-      <c r="C38" s="78" t="s">
-        <v>76</v>
-      </c>
-      <c r="D38" s="79"/>
-      <c r="E38" s="79"/>
-      <c r="F38" s="79"/>
-      <c r="G38" s="79"/>
-      <c r="H38" s="79"/>
-      <c r="I38" s="79"/>
-      <c r="J38" s="79"/>
-      <c r="K38" s="79"/>
-      <c r="L38" s="79"/>
-      <c r="M38" s="79"/>
-      <c r="N38" s="79"/>
-      <c r="O38" s="79"/>
-      <c r="P38" s="79"/>
-      <c r="Q38" s="79"/>
-      <c r="R38" s="80"/>
+      <c r="C38" s="79" t="s">
+        <v>75</v>
+      </c>
+      <c r="D38" s="80"/>
+      <c r="E38" s="80"/>
+      <c r="F38" s="80"/>
+      <c r="G38" s="80"/>
+      <c r="H38" s="80"/>
+      <c r="I38" s="80"/>
+      <c r="J38" s="80"/>
+      <c r="K38" s="80"/>
+      <c r="L38" s="80"/>
+      <c r="M38" s="80"/>
+      <c r="N38" s="80"/>
+      <c r="O38" s="80"/>
+      <c r="P38" s="80"/>
+      <c r="Q38" s="80"/>
+      <c r="R38" s="81"/>
     </row>
     <row r="39" spans="1:18">
       <c r="A39" s="51" t="str">
@@ -3253,8 +3256,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R30"/>
   <sheetViews>
-    <sheetView showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -3306,22 +3309,22 @@
         <v>9</v>
       </c>
       <c r="M3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="N3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N3" s="3" t="s">
+      <c r="O3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O3" s="3" t="s">
+      <c r="P3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P3" s="3" t="s">
+      <c r="Q3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="Q3" s="3" t="s">
+      <c r="R3" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="R3" s="3" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:18">
@@ -3330,7 +3333,7 @@
         <v>0000</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D4" s="18" t="s">
         <v>1</v>
@@ -3341,19 +3344,19 @@
       <c r="F4" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="15" t="s">
-        <v>4</v>
+      <c r="G4" s="70" t="s">
+        <v>77</v>
       </c>
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
       <c r="K4" s="35" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L4" s="36"/>
       <c r="M4" s="36"/>
       <c r="N4" s="37"/>
       <c r="O4" s="38" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P4" s="39"/>
       <c r="Q4" s="39"/>
@@ -3361,30 +3364,30 @@
     </row>
     <row r="6" spans="1:18">
       <c r="C6" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F6" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="H6" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="I6" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="G6" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="H6" s="12" t="s">
+      <c r="J6" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="I6" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="J6" s="13" t="s">
-        <v>33</v>
-      </c>
       <c r="K6" s="23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L6" s="24"/>
       <c r="M6" s="25"/>
       <c r="N6" s="19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="O6" s="6"/>
       <c r="P6" s="6"/>
@@ -3413,29 +3416,29 @@
         <v>0000</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D8" s="14"/>
       <c r="E8" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="F8" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="F8" s="16" t="s">
-        <v>39</v>
-      </c>
       <c r="G8" s="32" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H8" s="33"/>
       <c r="I8" s="33"/>
       <c r="J8" s="34"/>
       <c r="K8" s="32" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L8" s="33"/>
       <c r="M8" s="33"/>
       <c r="N8" s="34"/>
       <c r="O8" s="32" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P8" s="33"/>
       <c r="Q8" s="33"/>
@@ -3447,25 +3450,25 @@
         <v>0010</v>
       </c>
       <c r="C9" s="44" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D9" s="45"/>
       <c r="E9" s="45"/>
       <c r="F9" s="46"/>
       <c r="G9" s="44" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H9" s="45"/>
       <c r="I9" s="45"/>
       <c r="J9" s="46"/>
       <c r="K9" s="44" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L9" s="45"/>
       <c r="M9" s="45"/>
       <c r="N9" s="46"/>
       <c r="O9" s="44" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="P9" s="45"/>
       <c r="Q9" s="45"/>
@@ -3477,25 +3480,25 @@
         <v>0020</v>
       </c>
       <c r="C10" s="41" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D10" s="42"/>
       <c r="E10" s="42"/>
       <c r="F10" s="43"/>
       <c r="G10" s="41" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H10" s="42"/>
       <c r="I10" s="42"/>
       <c r="J10" s="43"/>
       <c r="K10" s="29" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L10" s="30"/>
       <c r="M10" s="30"/>
       <c r="N10" s="31"/>
       <c r="O10" s="29" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="P10" s="30"/>
       <c r="Q10" s="30"/>
@@ -3507,19 +3510,19 @@
         <v>0030</v>
       </c>
       <c r="C11" s="29" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D11" s="30"/>
       <c r="E11" s="30"/>
       <c r="F11" s="31"/>
       <c r="G11" s="29" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H11" s="30"/>
       <c r="I11" s="30"/>
       <c r="J11" s="31"/>
       <c r="K11" s="29" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L11" s="30"/>
       <c r="M11" s="30"/>
@@ -3535,25 +3538,25 @@
         <v>0040</v>
       </c>
       <c r="C12" s="20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D12" s="21"/>
       <c r="E12" s="21"/>
       <c r="F12" s="22"/>
       <c r="G12" s="20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H12" s="21"/>
       <c r="I12" s="21"/>
       <c r="J12" s="22"/>
       <c r="K12" s="20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L12" s="21"/>
       <c r="M12" s="21"/>
       <c r="N12" s="22"/>
       <c r="O12" s="20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="P12" s="21"/>
       <c r="Q12" s="21"/>
@@ -3565,25 +3568,25 @@
         <v>0050</v>
       </c>
       <c r="C13" s="26" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D13" s="27"/>
       <c r="E13" s="27"/>
       <c r="F13" s="28"/>
       <c r="G13" s="26" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H13" s="27"/>
       <c r="I13" s="27"/>
       <c r="J13" s="28"/>
       <c r="K13" s="26" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L13" s="27"/>
       <c r="M13" s="27"/>
       <c r="N13" s="28"/>
       <c r="O13" s="26" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="P13" s="27"/>
       <c r="Q13" s="27"/>
@@ -3989,7 +3992,7 @@
     <row r="1" spans="1:18" ht="9.9499999999999993" customHeight="1"/>
     <row r="2" spans="1:18">
       <c r="C2" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:18">
@@ -4024,22 +4027,22 @@
         <v>9</v>
       </c>
       <c r="M3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="N3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N3" s="3" t="s">
+      <c r="O3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O3" s="3" t="s">
+      <c r="P3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P3" s="3" t="s">
+      <c r="Q3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="Q3" s="3" t="s">
+      <c r="R3" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="R3" s="3" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:18">

</xml_diff>